<commit_message>
Update elec sector spending allocation to ISIC code files
</commit_message>
<xml_diff>
--- a/InputData/elec/SoTCCbIC/Share of Transmission Capital Costs by ISIC Code.xlsx
+++ b/InputData/elec/SoTCCbIC/Share of Transmission Capital Costs by ISIC Code.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\elec\SoTCCbIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\elec\SoTCCbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F09CD25-8B6A-452A-AF86-A50ACEAB6F77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="150" windowWidth="25665" windowHeight="16830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="150" windowWidth="25665" windowHeight="16830"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Cost Breakdowns" sheetId="1" r:id="rId3"/>
     <sheet name="SoTCCbIC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -486,7 +485,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
@@ -765,19 +764,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -870,13 +863,22 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_DefaultData" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal_DefaultData" xfId="5"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1154,45 +1156,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="61.85546875" customWidth="1"/>
+    <col min="2" max="2" width="61.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
         <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="14">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B4" s="12">
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B6" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>73</v>
       </c>
@@ -1203,34 +1205,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="77.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="77.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.73046875" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1238,7 +1240,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -1246,7 +1248,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -1254,7 +1256,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -1262,7 +1264,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1270,7 +1272,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1280,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1286,7 +1288,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1294,7 +1296,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1302,7 +1304,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1310,7 +1312,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -1318,7 +1320,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -1326,7 +1328,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1334,7 +1336,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>134</v>
       </c>
@@ -1342,7 +1344,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -1350,7 +1352,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -1358,7 +1360,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -1366,7 +1368,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1374,7 +1376,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1382,7 +1384,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1390,7 +1392,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1398,7 +1400,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1406,7 +1408,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1414,7 +1416,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1422,7 +1424,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>142</v>
       </c>
@@ -1430,7 +1432,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>144</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -1446,7 +1448,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1454,7 +1456,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1462,7 +1464,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1470,7 +1472,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -1478,7 +1480,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1486,7 +1488,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -1494,7 +1496,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1502,7 +1504,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1510,7 +1512,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1518,7 +1520,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -1526,7 +1528,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1534,7 +1536,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1542,7 +1544,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -1550,7 +1552,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -1558,7 +1560,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -1572,45 +1574,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="74" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="74.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.59765625" customWidth="1"/>
+    <col min="7" max="7" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="23.1328125" customWidth="1"/>
+    <col min="11" max="11" width="74.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-    </row>
-    <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="52"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+    </row>
+    <row r="2" spans="1:6" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="47" t="s">
         <v>122</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1623,954 +1625,957 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="34">
         <v>375000</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="45">
         <f>B4/$B$52</f>
         <v>1.2997394453391755E-2</v>
       </c>
-      <c r="D4" s="10" t="str">
+      <c r="D4" s="8" t="str">
         <f>'OECD Mapping'!A37</f>
         <v>D68: Real estate activities</v>
       </c>
-      <c r="E4" s="10" t="str">
+      <c r="E4" s="8" t="str">
         <f>'OECD Mapping'!B37</f>
         <v>ISIC 68</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="F4" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="34">
         <v>363636.36363636365</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="45">
         <f t="shared" ref="C5:C49" si="0">B5/$B$52</f>
         <v>1.2603534015410187E-2</v>
       </c>
-      <c r="D5" s="11" t="str">
+      <c r="D5" s="9" t="str">
         <f>'OECD Mapping'!A37</f>
         <v>D68: Real estate activities</v>
       </c>
-      <c r="E5" s="11" t="str">
+      <c r="E5" s="9" t="str">
         <f>'OECD Mapping'!B37</f>
         <v>ISIC 68</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="F5" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="34">
         <v>900000</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="45">
         <f t="shared" si="0"/>
         <v>3.1193746688140213E-2</v>
       </c>
-      <c r="D6" s="10" t="str">
+      <c r="D6" s="8" t="str">
         <f>'OECD Mapping'!A38</f>
         <v>D69T82: Other business sector services</v>
       </c>
-      <c r="E6" s="10" t="str">
+      <c r="E6" s="8" t="str">
         <f>'OECD Mapping'!B38</f>
         <v>ISIC 69T82</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="F6" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="34">
         <v>675000</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="45">
         <f t="shared" si="0"/>
         <v>2.3395310016105158E-2</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="D7" s="8" t="str">
         <f>'OECD Mapping'!A38</f>
         <v>D69T82: Other business sector services</v>
       </c>
-      <c r="E7" s="10" t="str">
+      <c r="E7" s="8" t="str">
         <f>'OECD Mapping'!B38</f>
         <v>ISIC 69T82</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="F7" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="34">
         <v>2313636.3636363638</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="C8" s="45"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="B9" s="33"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="38">
+      <c r="B11" s="36">
         <v>600000</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="45">
         <f t="shared" si="0"/>
         <v>2.0795831125426809E-2</v>
       </c>
-      <c r="D11" s="10" t="str">
+      <c r="D11" s="8" t="str">
         <f>'OECD Mapping'!A16</f>
         <v>D239: Cement and other nometallic minerals</v>
       </c>
-      <c r="E11" s="10" t="str">
+      <c r="E11" s="8" t="str">
         <f>'OECD Mapping'!B16</f>
         <v>ISIC 239</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="F11" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="38">
+      <c r="B12" s="36">
         <v>4950000</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="45">
         <f t="shared" si="0"/>
         <v>0.17156560678477117</v>
       </c>
-      <c r="D12" s="10" t="str">
+      <c r="D12" s="8" t="str">
         <f>'OECD Mapping'!A19</f>
         <v>D25: Fabricated metal products</v>
       </c>
-      <c r="E12" s="10" t="str">
+      <c r="E12" s="8" t="str">
         <f>'OECD Mapping'!B19</f>
         <v>ISIC 25</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="F12" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="38">
+      <c r="B13" s="36">
         <v>3300000</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="45">
         <f t="shared" si="0"/>
         <v>0.11437707118984744</v>
       </c>
-      <c r="D13" s="12" t="str">
+      <c r="D13" s="10" t="str">
         <f>'OECD Mapping'!A21</f>
         <v>D27: Electrical equipment</v>
       </c>
-      <c r="E13" s="12" t="str">
+      <c r="E13" s="10" t="str">
         <f>'OECD Mapping'!B21</f>
         <v>ISIC 27</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="F13" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="37">
         <v>8850000</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="C14" s="45"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="B15" s="38"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="13" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="36">
         <v>1765400.1798561153</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="45">
         <f t="shared" si="0"/>
         <v>6.1188273348476478E-2</v>
       </c>
-      <c r="D16" s="4" t="str">
+      <c r="D16" s="54" t="str">
         <f>'OECD Mapping'!A29</f>
         <v>D41T43: Construction</v>
       </c>
-      <c r="E16" s="4" t="str">
+      <c r="E16" s="54" t="str">
         <f>'OECD Mapping'!B29</f>
         <v>ISIC 41T43</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="F16" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="38">
+      <c r="B17" s="36">
         <v>3276000</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="45">
         <f t="shared" si="0"/>
         <v>0.11354523794483037</v>
       </c>
-      <c r="D17" s="4" t="str">
+      <c r="D17" s="54" t="str">
         <f>'OECD Mapping'!A29</f>
         <v>D41T43: Construction</v>
       </c>
-      <c r="E17" s="4" t="str">
+      <c r="E17" s="54" t="str">
         <f>'OECD Mapping'!B29</f>
         <v>ISIC 41T43</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24" t="s">
+      <c r="F17" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="39">
+      <c r="B18" s="37">
         <v>5041400.179856115</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+      <c r="C18" s="45"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="41">
+      <c r="B19" s="39">
         <v>16205036.543492477</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+      <c r="C19" s="45"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="39">
+      <c r="B22" s="37">
         <v>1800000</v>
       </c>
-      <c r="C22" s="47">
+      <c r="C22" s="45">
         <f t="shared" si="0"/>
         <v>6.2387493376280426E-2</v>
       </c>
-      <c r="D22" s="4" t="str">
-        <f>'OECD Mapping'!A26</f>
-        <v>D351: Electricity generation and distribution</v>
-      </c>
-      <c r="E22" s="10" t="str">
-        <f>'OECD Mapping'!B26</f>
-        <v>ISIC 351</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="s">
+      <c r="D22" s="3" t="str">
+        <f>'OECD Mapping'!$A$21</f>
+        <v>D27: Electrical equipment</v>
+      </c>
+      <c r="E22" s="8" t="str">
+        <f>'OECD Mapping'!$B$21</f>
+        <v>ISIC 27</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="43">
+      <c r="B23" s="41">
         <v>650000</v>
       </c>
-      <c r="C23" s="47">
+      <c r="C23" s="45">
         <f t="shared" si="0"/>
         <v>2.2528817052545707E-2</v>
       </c>
-      <c r="D23" s="4" t="str">
-        <f>'OECD Mapping'!A22</f>
-        <v>D28: Machinery and equipment, nec</v>
-      </c>
-      <c r="E23" s="10" t="str">
-        <f>'OECD Mapping'!B22</f>
-        <v>ISIC 28</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28" t="s">
+      <c r="D23" s="3" t="str">
+        <f>'OECD Mapping'!$A$21</f>
+        <v>D27: Electrical equipment</v>
+      </c>
+      <c r="E23" s="8" t="str">
+        <f>'OECD Mapping'!$B$21</f>
+        <v>ISIC 27</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="43">
+      <c r="B24" s="41">
         <v>20000</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="45">
         <f t="shared" si="0"/>
         <v>6.9319437084756029E-4</v>
       </c>
-      <c r="D24" s="4" t="str">
-        <f>'OECD Mapping'!A22</f>
-        <v>D28: Machinery and equipment, nec</v>
-      </c>
-      <c r="E24" s="11" t="str">
-        <f>'OECD Mapping'!B22</f>
-        <v>ISIC 28</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
+      <c r="D24" s="3" t="str">
+        <f>'OECD Mapping'!$A$21</f>
+        <v>D27: Electrical equipment</v>
+      </c>
+      <c r="E24" s="8" t="str">
+        <f>'OECD Mapping'!$B$21</f>
+        <v>ISIC 27</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="39">
+      <c r="B25" s="37">
         <v>4800000</v>
       </c>
-      <c r="C25" s="47">
+      <c r="C25" s="45">
         <f t="shared" si="0"/>
         <v>0.16636664900341447</v>
       </c>
-      <c r="D25" s="4" t="str">
-        <f>'OECD Mapping'!A21</f>
+      <c r="D25" s="3" t="str">
+        <f>'OECD Mapping'!$A$21</f>
         <v>D27: Electrical equipment</v>
       </c>
-      <c r="E25" s="10" t="str">
-        <f>'OECD Mapping'!B21</f>
+      <c r="E25" s="8" t="str">
+        <f>'OECD Mapping'!$B$21</f>
         <v>ISIC 27</v>
       </c>
-      <c r="F25" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="28" t="s">
+      <c r="F25" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="43">
-        <v>0</v>
-      </c>
-      <c r="C26" s="47">
+      <c r="B26" s="41">
+        <v>0</v>
+      </c>
+      <c r="C26" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D26" s="4" t="str">
-        <f>'OECD Mapping'!A21</f>
+      <c r="D26" s="3" t="str">
+        <f>'OECD Mapping'!$A$21</f>
         <v>D27: Electrical equipment</v>
       </c>
-      <c r="E26" s="10" t="str">
-        <f>'OECD Mapping'!B21</f>
+      <c r="E26" s="8" t="str">
+        <f>'OECD Mapping'!$B$21</f>
         <v>ISIC 27</v>
       </c>
-      <c r="F26" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
+      <c r="F26" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="39">
+      <c r="B27" s="37">
         <v>7270000</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25" t="s">
+      <c r="C27" s="45"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="47">
+      <c r="B28" s="38"/>
+      <c r="C28" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24" t="s">
+      <c r="D28" s="3"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A29" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="39">
+      <c r="B29" s="37">
         <v>2092500</v>
       </c>
-      <c r="C29" s="47">
+      <c r="C29" s="45">
         <f t="shared" si="0"/>
         <v>7.2525461049925993E-2</v>
       </c>
-      <c r="D29" s="10" t="str">
+      <c r="D29" s="8" t="str">
         <f>'OECD Mapping'!$A$29</f>
         <v>D41T43: Construction</v>
       </c>
-      <c r="E29" s="10" t="str">
+      <c r="E29" s="8" t="str">
         <f>'OECD Mapping'!$B$29</f>
         <v>ISIC 41T43</v>
       </c>
-      <c r="F29" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="28" t="s">
+      <c r="F29" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A30" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="43">
+      <c r="B30" s="41">
         <v>744000</v>
       </c>
-      <c r="C30" s="47">
+      <c r="C30" s="45">
         <f t="shared" si="0"/>
         <v>2.5786830595529241E-2</v>
       </c>
-      <c r="D30" s="10" t="str">
+      <c r="D30" s="8" t="str">
         <f>'OECD Mapping'!$A$29</f>
         <v>D41T43: Construction</v>
       </c>
-      <c r="E30" s="11" t="str">
+      <c r="E30" s="9" t="str">
         <f>'OECD Mapping'!$B$29</f>
         <v>ISIC 41T43</v>
       </c>
-      <c r="F30" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="28" t="s">
+      <c r="F30" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="43">
+      <c r="B31" s="41">
         <v>27900</v>
       </c>
-      <c r="C31" s="47">
+      <c r="C31" s="45">
         <f t="shared" si="0"/>
         <v>9.6700614733234659E-4</v>
       </c>
-      <c r="D31" s="10" t="str">
+      <c r="D31" s="8" t="str">
         <f>'OECD Mapping'!$A$29</f>
         <v>D41T43: Construction</v>
       </c>
-      <c r="E31" s="10" t="str">
+      <c r="E31" s="8" t="str">
         <f>'OECD Mapping'!$B$29</f>
         <v>ISIC 41T43</v>
       </c>
-      <c r="F31" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="23" t="s">
+      <c r="F31" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A32" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="38">
-        <v>0</v>
-      </c>
-      <c r="C32" s="47">
+      <c r="B32" s="36">
+        <v>0</v>
+      </c>
+      <c r="C32" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D32" s="10" t="str">
+      <c r="D32" s="8" t="str">
         <f>'OECD Mapping'!$A$29</f>
         <v>D41T43: Construction</v>
       </c>
-      <c r="E32" s="10" t="str">
+      <c r="E32" s="8" t="str">
         <f>'OECD Mapping'!$B$29</f>
         <v>ISIC 41T43</v>
       </c>
-      <c r="F32" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23" t="s">
+      <c r="F32" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A33" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="38">
-        <v>0</v>
-      </c>
-      <c r="C33" s="47">
+      <c r="B33" s="36">
+        <v>0</v>
+      </c>
+      <c r="C33" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D33" s="10" t="str">
+      <c r="D33" s="8" t="str">
         <f>'OECD Mapping'!$A$29</f>
         <v>D41T43: Construction</v>
       </c>
-      <c r="E33" s="11" t="str">
+      <c r="E33" s="9" t="str">
         <f>'OECD Mapping'!$B$29</f>
         <v>ISIC 41T43</v>
       </c>
-      <c r="F33" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
+      <c r="F33" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A34" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="39">
+      <c r="B34" s="37">
         <v>2864400</v>
       </c>
-      <c r="C34" s="47"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
+      <c r="C34" s="45"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="42">
+      <c r="B35" s="40">
         <v>10134400</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
+      <c r="C35" s="45"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A36" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25" t="s">
+      <c r="C36" s="45"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A37" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
+      <c r="B37" s="38"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A38" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="39">
+      <c r="B38" s="37">
         <v>375000</v>
       </c>
-      <c r="C38" s="47">
+      <c r="C38" s="45">
         <f t="shared" si="0"/>
         <v>1.2997394453391755E-2</v>
       </c>
-      <c r="D38" s="4" t="str">
+      <c r="D38" s="3" t="str">
         <f>'OECD Mapping'!A38</f>
         <v>D69T82: Other business sector services</v>
       </c>
-      <c r="E38" s="10" t="str">
+      <c r="E38" s="8" t="str">
         <f>'OECD Mapping'!B38</f>
         <v>ISIC 69T82</v>
       </c>
-      <c r="F38" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
+      <c r="F38" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A39" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="39">
+      <c r="B39" s="37">
         <v>750000</v>
       </c>
-      <c r="C39" s="47">
+      <c r="C39" s="45">
         <f t="shared" si="0"/>
         <v>2.5994788906783511E-2</v>
       </c>
-      <c r="D39" s="50" t="str">
+      <c r="D39" s="48" t="str">
         <f>'OECD Mapping'!A38</f>
         <v>D69T82: Other business sector services</v>
       </c>
-      <c r="E39" s="11" t="str">
+      <c r="E39" s="9" t="str">
         <f>'OECD Mapping'!B38</f>
         <v>ISIC 69T82</v>
       </c>
-      <c r="F39" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24" t="s">
+      <c r="F39" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="39">
+      <c r="B40" s="37">
         <v>1125000</v>
       </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="27" t="s">
+      <c r="C40" s="45"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A41" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="42"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24" t="s">
+      <c r="B41" s="40"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A42" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="39">
+      <c r="B42" s="37">
         <v>222000</v>
       </c>
-      <c r="C42" s="47">
+      <c r="C42" s="45">
         <f t="shared" si="0"/>
         <v>7.6944575164079191E-3</v>
       </c>
-      <c r="D42" s="50" t="str">
+      <c r="D42" s="48" t="str">
         <f>'OECD Mapping'!A38</f>
         <v>D69T82: Other business sector services</v>
       </c>
-      <c r="E42" s="11" t="str">
+      <c r="E42" s="9" t="str">
         <f>'OECD Mapping'!B38</f>
         <v>ISIC 69T82</v>
       </c>
-      <c r="F42" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="24" t="s">
+      <c r="F42" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A43" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="39">
+      <c r="B43" s="37">
         <v>1110000</v>
       </c>
-      <c r="C43" s="47">
+      <c r="C43" s="45">
         <f t="shared" si="0"/>
         <v>3.8472287582039591E-2</v>
       </c>
-      <c r="D43" s="50" t="str">
+      <c r="D43" s="48" t="str">
         <f>'OECD Mapping'!A38</f>
         <v>D69T82: Other business sector services</v>
       </c>
-      <c r="E43" s="10" t="str">
+      <c r="E43" s="8" t="str">
         <f>'OECD Mapping'!B38</f>
         <v>ISIC 69T82</v>
       </c>
-      <c r="F43" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="24" t="s">
+      <c r="F43" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A44" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="39">
+      <c r="B44" s="37">
         <v>1332000</v>
       </c>
-      <c r="C44" s="47"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="27" t="s">
+      <c r="C44" s="45"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A45" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="42"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="23" t="s">
+      <c r="B45" s="40"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A46" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="B46" s="38">
-        <v>0</v>
-      </c>
-      <c r="C46" s="47">
+      <c r="B46" s="36">
+        <v>0</v>
+      </c>
+      <c r="C46" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D46" s="50" t="str">
+      <c r="D46" s="48" t="str">
         <f>'OECD Mapping'!$A$38</f>
         <v>D69T82: Other business sector services</v>
       </c>
-      <c r="E46" s="10" t="str">
+      <c r="E46" s="8" t="str">
         <f>'OECD Mapping'!$B$38</f>
         <v>ISIC 69T82</v>
       </c>
-      <c r="F46" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23" t="s">
+      <c r="F46" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A47" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="B47" s="38">
-        <v>0</v>
-      </c>
-      <c r="C47" s="47">
+      <c r="B47" s="36">
+        <v>0</v>
+      </c>
+      <c r="C47" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D47" s="50" t="str">
+      <c r="D47" s="48" t="str">
         <f>'OECD Mapping'!$A$38</f>
         <v>D69T82: Other business sector services</v>
       </c>
-      <c r="E47" s="10" t="str">
+      <c r="E47" s="8" t="str">
         <f>'OECD Mapping'!$B$38</f>
         <v>ISIC 69T82</v>
       </c>
-      <c r="F47" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="23" t="s">
+      <c r="F47" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A48" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="B48" s="38">
-        <v>0</v>
-      </c>
-      <c r="C48" s="47">
+      <c r="B48" s="36">
+        <v>0</v>
+      </c>
+      <c r="C48" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D48" s="50" t="str">
+      <c r="D48" s="48" t="str">
         <f>'OECD Mapping'!$A$38</f>
         <v>D69T82: Other business sector services</v>
       </c>
-      <c r="E48" s="11" t="str">
+      <c r="E48" s="9" t="str">
         <f>'OECD Mapping'!$B$38</f>
         <v>ISIC 69T82</v>
       </c>
-      <c r="F48" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="29" t="s">
+      <c r="F48" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A49" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B49" s="38">
+      <c r="B49" s="36">
         <v>55500</v>
       </c>
-      <c r="C49" s="47">
+      <c r="C49" s="45">
         <f t="shared" si="0"/>
         <v>1.9236143791019798E-3</v>
       </c>
-      <c r="D49" s="50" t="str">
+      <c r="D49" s="48" t="str">
         <f>'OECD Mapping'!A36</f>
         <v>D64T66: Financial and insurance activities</v>
       </c>
-      <c r="E49" s="10" t="str">
+      <c r="E49" s="8" t="str">
         <f>'OECD Mapping'!B36</f>
         <v>ISIC 64T66</v>
       </c>
-      <c r="F49" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="23" t="s">
+      <c r="F49" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A50" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="B50" s="38">
+      <c r="B50" s="36">
         <v>55500</v>
       </c>
-      <c r="C50" s="47"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="30" t="s">
+      <c r="C50" s="45"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A51" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="B51" s="44">
+      <c r="B51" s="42">
         <v>2512500</v>
       </c>
-      <c r="C51" s="47"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="31" t="s">
+      <c r="C51" s="45"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A52" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="45">
+      <c r="B52" s="43">
         <v>28851936.543492477</v>
       </c>
-      <c r="C52" s="47"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="32" t="s">
+      <c r="C52" s="45"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A53" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="46">
+      <c r="B53" s="44">
         <v>1007500</v>
       </c>
-      <c r="C53" s="47"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+      <c r="C53" s="45"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="B54" s="33">
+      <c r="B54" s="31">
         <v>29859436.543492477</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="48"/>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C55" s="46"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C56" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2582,7 +2587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -2590,321 +2595,321 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="26" width="10.42578125" customWidth="1"/>
-    <col min="27" max="27" width="13.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.28515625" customWidth="1"/>
-    <col min="29" max="43" width="10.42578125" customWidth="1"/>
+    <col min="2" max="26" width="10.3984375" customWidth="1"/>
+    <col min="27" max="27" width="13.265625" customWidth="1"/>
+    <col min="28" max="28" width="11.265625" customWidth="1"/>
+    <col min="29" max="43" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A1" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="51" t="s">
+      <c r="N1" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="51" t="s">
+      <c r="O1" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="P1" s="51" t="s">
+      <c r="P1" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="Q1" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="R1" s="51" t="s">
+      <c r="R1" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="S1" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="51" t="s">
+      <c r="U1" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="51" t="s">
+      <c r="V1" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="51" t="s">
+      <c r="W1" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="51" t="s">
+      <c r="X1" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" s="51" t="s">
+      <c r="Y1" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="51" t="s">
+      <c r="Z1" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="AA1" s="51" t="s">
+      <c r="AA1" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="AB1" s="51" t="s">
+      <c r="AB1" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="AC1" s="51" t="s">
+      <c r="AC1" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" s="51" t="s">
+      <c r="AD1" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" s="51" t="s">
+      <c r="AE1" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="AF1" s="51" t="s">
+      <c r="AF1" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="AG1" s="51" t="s">
+      <c r="AG1" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="AH1" s="51" t="s">
+      <c r="AH1" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="AI1" s="51" t="s">
+      <c r="AI1" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="AJ1" s="51" t="s">
+      <c r="AJ1" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="AK1" s="51" t="s">
+      <c r="AK1" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="AL1" s="51" t="s">
+      <c r="AL1" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="AM1" s="51" t="s">
+      <c r="AM1" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="AN1" s="51" t="s">
+      <c r="AN1" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="AO1" s="51" t="s">
+      <c r="AO1" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="AP1" s="51" t="s">
+      <c r="AP1" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="AQ1" s="51" t="s">
+      <c r="AQ1" s="49" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!B$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!C$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!D$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!E$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!F$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!G$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!H$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!I$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!J$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!K$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!L$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!M$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!N$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!O$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!P$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>2.0795831125426809E-2</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!Q$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="R2" s="13">
+      <c r="R2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!R$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="S2" s="13">
+      <c r="S2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!S$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0.17156560678477117</v>
       </c>
-      <c r="T2" s="13">
+      <c r="T2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!T$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="U2" s="13">
+      <c r="U2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!U$1,'Cost Breakdowns'!$C$3:$C$49)</f>
-        <v>0.28074372019326188</v>
-      </c>
-      <c r="V2" s="13">
+        <v>0.3663532249929356</v>
+      </c>
+      <c r="V2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!V$1,'Cost Breakdowns'!$C$3:$C$49)</f>
-        <v>2.3222011423393266E-2</v>
-      </c>
-      <c r="W2" s="13">
+        <v>0</v>
+      </c>
+      <c r="W2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!W$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="X2" s="13">
+      <c r="X2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!X$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="Y2" s="13">
+      <c r="Y2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!Y$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="Z2" s="13">
+      <c r="Z2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!Z$1,'Cost Breakdowns'!$C$3:$C$49)</f>
-        <v>6.2387493376280426E-2</v>
-      </c>
-      <c r="AA2" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AA$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="13">
+      <c r="AB2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AB$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AC2" s="13">
+      <c r="AC2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AC$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0.27401280908609443</v>
       </c>
-      <c r="AD2" s="13">
+      <c r="AD2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AD$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AE2" s="13">
+      <c r="AE2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AE$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AF2" s="13">
+      <c r="AF2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AF$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AG2" s="13">
+      <c r="AG2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AG$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AH2" s="13">
+      <c r="AH2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AH$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AI2" s="13">
+      <c r="AI2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AI$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AJ2" s="13">
+      <c r="AJ2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AJ$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>1.9236143791019798E-3</v>
       </c>
-      <c r="AK2" s="13">
+      <c r="AK2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AK$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>2.5600928468801944E-2</v>
       </c>
-      <c r="AL2" s="13">
+      <c r="AL2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AL$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0.13974798516286813</v>
       </c>
-      <c r="AM2" s="13">
+      <c r="AM2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AM$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AN2" s="13">
+      <c r="AN2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AN$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AO2" s="13">
+      <c r="AO2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AO$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AP2" s="13">
+      <c r="AP2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AP$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
-      <c r="AQ2" s="13">
+      <c r="AQ2" s="11">
         <f>SUMIF('Cost Breakdowns'!$E$3:$E$49,SoTCCbIC!AQ$1,'Cost Breakdowns'!$C$3:$C$49)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="F10" s="13"/>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="F10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>